<commit_message>
Atualizando a planilha Excel
</commit_message>
<xml_diff>
--- a/bases/PlanilhasExcel.xlsx
+++ b/bases/PlanilhasExcel.xlsx
@@ -14,45 +14,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Mês</t>
-  </si>
-  <si>
-    <t>Produto</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Fev</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Arroz</t>
-  </si>
-  <si>
-    <t>Qtd</t>
-  </si>
-  <si>
-    <t>Feijao</t>
-  </si>
-  <si>
-    <t>Sal</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+  <si>
+    <t>id_paciente</t>
+  </si>
+  <si>
+    <t>nome do paciente</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>idade</t>
+  </si>
+  <si>
+    <t>Homens da Carolina</t>
+  </si>
+  <si>
+    <t>Hospitais</t>
+  </si>
+  <si>
+    <t>Hipertens</t>
+  </si>
+  <si>
+    <t>Felipe Roch</t>
+  </si>
+  <si>
+    <t>Hospital São José</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Asma</t>
+  </si>
+  <si>
+    <t>Gustavo Ramos</t>
+  </si>
+  <si>
+    <t>Hospital Sa</t>
+  </si>
+  <si>
+    <t>Cardiopatia</t>
+  </si>
+  <si>
+    <t>Bianca Araújo</t>
+  </si>
+  <si>
+    <t>Hospitalar</t>
+  </si>
+  <si>
+    <t>Rafael Barbosa</t>
+  </si>
+  <si>
+    <t>Artrite</t>
+  </si>
+  <si>
+    <t>Hospital E</t>
+  </si>
+  <si>
+    <t>Enxa</t>
+  </si>
+  <si>
+    <t>Tiago Ca</t>
+  </si>
+  <si>
+    <t>Osteo</t>
+  </si>
+  <si>
+    <t>Vanessa Teix</t>
+  </si>
+  <si>
+    <t>Depressão</t>
+  </si>
+  <si>
+    <t>Eduardo Oliveira</t>
+  </si>
+  <si>
+    <t>Hospi</t>
+  </si>
+  <si>
+    <t>Insônia</t>
+  </si>
+  <si>
+    <t>Quadro</t>
+  </si>
+  <si>
+    <t>Pedro Santos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,6 +122,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,19 +147,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,75 +459,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2">
+        <v>53</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>55</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>15</v>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alterando dados na planilha excel
</commit_message>
<xml_diff>
--- a/bases/PlanilhasExcel.xlsx
+++ b/bases/PlanilhasExcel.xlsx
@@ -14,99 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id_paciente</t>
   </si>
   <si>
-    <t>nome do paciente</t>
-  </si>
-  <si>
-    <t>hospital</t>
-  </si>
-  <si>
-    <t>idade</t>
-  </si>
-  <si>
-    <t>Homens da Carolina</t>
-  </si>
-  <si>
-    <t>Hospitais</t>
-  </si>
-  <si>
-    <t>Hipertens</t>
-  </si>
-  <si>
-    <t>Felipe Roch</t>
-  </si>
-  <si>
-    <t>Hospital São José</t>
-  </si>
-  <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Hospital</t>
-  </si>
-  <si>
-    <t>Asma</t>
-  </si>
-  <si>
-    <t>Gustavo Ramos</t>
-  </si>
-  <si>
-    <t>Hospital Sa</t>
-  </si>
-  <si>
-    <t>Cardiopatia</t>
-  </si>
-  <si>
-    <t>Bianca Araújo</t>
-  </si>
-  <si>
-    <t>Hospitalar</t>
-  </si>
-  <si>
-    <t>Rafael Barbosa</t>
-  </si>
-  <si>
-    <t>Artrite</t>
-  </si>
-  <si>
-    <t>Hospital E</t>
-  </si>
-  <si>
-    <t>Enxa</t>
-  </si>
-  <si>
-    <t>Tiago Ca</t>
-  </si>
-  <si>
-    <t>Osteo</t>
-  </si>
-  <si>
-    <t>Vanessa Teix</t>
-  </si>
-  <si>
-    <t>Depressão</t>
-  </si>
-  <si>
-    <t>Eduardo Oliveira</t>
-  </si>
-  <si>
-    <t>Hospi</t>
-  </si>
-  <si>
-    <t>Insônia</t>
-  </si>
-  <si>
-    <t>Quadro</t>
-  </si>
-  <si>
-    <t>Pedro Santos</t>
+    <t>id_prescricao</t>
+  </si>
+  <si>
+    <t>nome_medicamento</t>
+  </si>
+  <si>
+    <t>dosagem</t>
+  </si>
+  <si>
+    <t>Lisinopril</t>
+  </si>
+  <si>
+    <t>10mg</t>
+  </si>
+  <si>
+    <t>Metformina</t>
+  </si>
+  <si>
+    <t>500mg</t>
+  </si>
+  <si>
+    <t>Salbutamol</t>
+  </si>
+  <si>
+    <t>100mcg</t>
+  </si>
+  <si>
+    <t>Atorvastatina</t>
+  </si>
+  <si>
+    <t>20mg</t>
   </si>
 </sst>
 </file>
@@ -462,7 +405,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,10 +419,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -487,179 +430,109 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>32</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>48</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>203</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>204</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2">
-        <v>53</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2">
-        <v>37</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>39</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>55</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="2">
-        <v>42</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>